<commit_message>
Meeting on 11/25/23 recorded
</commit_message>
<xml_diff>
--- a/src/main/resources/Meetings.xlsx
+++ b/src/main/resources/Meetings.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Megac\Documents\College\CSCI\DobolyiCompSci\MegacWasTaken-project3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Megac\Documents\College\CSCI\DobolyiCompSci\MegacWasTaken-project3\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0096B96-E522-4B38-8B9F-9F88365F88B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55DA3882-12C7-43E7-829A-E610B1D95A25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5628" yWindow="2760" windowWidth="23040" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="4">
   <si>
     <t>Date</t>
   </si>
@@ -303,7 +303,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -356,6 +356,12 @@
       <c r="A5" s="2">
         <v>45255</v>
       </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2">

</xml_diff>

<commit_message>
ta feedback, meetings, and requirements final push
</commit_message>
<xml_diff>
--- a/src/main/resources/Meetings.xlsx
+++ b/src/main/resources/Meetings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Megac\Documents\College\CSCI\DobolyiCompSci\MegacWasTaken-project3\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{103570AD-5EFC-442D-A408-E38D208AAD35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4092F24A-103B-4ADE-81D9-4CFCC15FE9E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5628" yWindow="2760" windowWidth="23040" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="4">
   <si>
     <t>Date</t>
   </si>
@@ -302,8 +302,8 @@
   </sheetPr>
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -400,6 +400,12 @@
       <c r="A9" s="3">
         <v>45269</v>
       </c>
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1" gridLines="1"/>

</xml_diff>